<commit_message>
Add tables names to excel sheets
</commit_message>
<xml_diff>
--- a/inputs/table_metadata.xlsx
+++ b/inputs/table_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect-my.sharepoint.com/personal/izaak_jephson_socialsecurity_gov_scot/Documents/R/dev/excel_output/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="749" documentId="8_{44357B8C-CE93-45F8-9847-28F6F3CFF9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDB25843-729C-4E78-864E-A4A0B9CBE4FC}"/>
+  <xr:revisionPtr revIDLastSave="750" documentId="8_{44357B8C-CE93-45F8-9847-28F6F3CFF9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84AEA740-1DCE-4AF1-9031-E2AD1A90912F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{02C0BD84-F639-494E-8800-A6BEC8DFBE50}"/>
+    <workbookView xWindow="13470" yWindow="-16470" windowWidth="29040" windowHeight="15840" xr2:uid="{02C0BD84-F639-494E-8800-A6BEC8DFBE50}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="365">
   <si>
     <t>sheet_number</t>
   </si>
@@ -485,9 +485,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>Adult Disability Payment from 21 March 2022 to 30 April 2024</t>
   </si>
   <si>
     <t>Table 1</t>
@@ -1562,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18806EA-A3C1-4EE2-9978-D5A5314A02E8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1584,7 +1581,7 @@
         <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1630,16 +1627,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1647,16 +1644,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1664,16 +1661,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1681,16 +1678,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1698,16 +1695,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1715,16 +1712,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1732,16 +1729,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1749,16 +1746,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1766,16 +1763,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1783,16 +1780,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1800,16 +1797,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1817,16 +1814,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1834,16 +1831,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1851,16 +1848,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1868,16 +1865,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1885,16 +1882,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1902,16 +1899,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1919,16 +1916,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1936,16 +1933,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1953,16 +1950,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1970,16 +1967,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1987,16 +1984,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -2004,16 +2001,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -2021,16 +2018,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -2038,16 +2035,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -2055,16 +2052,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2098,242 +2095,242 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -3957,7 +3954,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -3965,7 +3962,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -3973,60 +3970,60 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -4034,410 +4031,410 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" t="s">
         <v>196</v>
-      </c>
-      <c r="B17" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B38" t="s">
         <v>238</v>
-      </c>
-      <c r="B38" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B39" t="s">
         <v>240</v>
-      </c>
-      <c r="B39" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" t="s">
         <v>244</v>
-      </c>
-      <c r="B41" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>247</v>
+      </c>
+      <c r="B43" t="s">
         <v>248</v>
-      </c>
-      <c r="B43" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>249</v>
+      </c>
+      <c r="B44" t="s">
         <v>250</v>
-      </c>
-      <c r="B44" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>251</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>253</v>
+      </c>
+      <c r="B46" t="s">
         <v>254</v>
-      </c>
-      <c r="B46" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>255</v>
+      </c>
+      <c r="B47" t="s">
         <v>256</v>
-      </c>
-      <c r="B47" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>257</v>
+      </c>
+      <c r="B48" t="s">
         <v>258</v>
-      </c>
-      <c r="B48" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>259</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>263</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>265</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>267</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>269</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>271</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>275</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>277</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -4449,7 +4446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EFF6D9-D772-4842-AAA7-9DD8E041DF58}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>